<commit_message>
few more changes to 500
</commit_message>
<xml_diff>
--- a/src/main/resources/Testcases.xlsx
+++ b/src/main/resources/Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristofer Radzinsh\PrimeAutomationRepository\prime-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6094EBB2-7761-46B7-981D-703DE80EA54B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D397F-0C4B-4844-A73C-D0D419AB4F3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="10690" windowWidth="21820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -962,7 +962,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>